<commit_message>
Analiza drzanja nastave funkcionalna po kolonama
</commit_message>
<xml_diff>
--- a/Novi_Izveštaj o radu_za_Nastavnike_Natasa_Bogdanovic.xlsx
+++ b/Novi_Izveštaj o radu_za_Nastavnike_Natasa_Bogdanovic.xlsx
@@ -5,12 +5,12 @@
   <workbookPr hidePivotFieldList="1" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://vtsnis-my.sharepoint.com/personal/milan_ristic_akademijanis_edu_rs/Documents/Projekti/PDF Generator radnih svezaka/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://vtsnis-my.sharepoint.com/personal/milan_ristic_akademijanis_edu_rs/Documents/Git folder za generator radnih svezaka/GeneratorRadnihSvezaka/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="25" documentId="8_{5A629DB8-CD87-4961-9FDE-2D66BA9658EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E0225CFC-85E8-47F8-9C89-7C299AF2F561}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="13_ncr:1_{515AE231-9F81-4BD4-8A77-B049EAC38BE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{970071BA-E47B-4D6B-9A4E-6C9BDB1B741D}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="2" activeTab="6" xr2:uid="{63FCCB33-4A62-4BAF-94D7-AE2680D11626}"/>
+    <workbookView xWindow="-4740" yWindow="-21720" windowWidth="38640" windowHeight="21120" firstSheet="2" activeTab="6" xr2:uid="{63FCCB33-4A62-4BAF-94D7-AE2680D11626}"/>
   </bookViews>
   <sheets>
     <sheet name="Osnovni podaci" sheetId="5" r:id="rId1"/>
@@ -2364,7 +2364,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="89">
+  <cellXfs count="86">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyFont="1"/>
@@ -2488,6 +2488,39 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" pivotButton="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="3"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="3"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -2500,42 +2533,6 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" pivotButton="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="3"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="3"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="20% - Accent3" xfId="4" builtinId="38"/>
@@ -2544,43 +2541,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Total" xfId="2" builtinId="25"/>
   </cellStyles>
-  <dxfs count="30">
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
+  <dxfs count="18">
     <dxf>
       <alignment wrapText="1"/>
     </dxf>
@@ -3012,10 +2973,6 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Excel Services" refreshedDate="45700.930710995373" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="460" xr:uid="{530C62FA-8687-4493-BDAF-577F166D3B65}">
   <cacheSource type="worksheet">
@@ -7887,7 +7844,7 @@
     <dataField name="Prosečan broj studenata" fld="7" subtotal="average" baseField="0" baseItem="0" numFmtId="1"/>
   </dataFields>
   <formats count="3">
-    <format dxfId="17">
+    <format dxfId="5">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="1">
@@ -7896,7 +7853,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="16">
+    <format dxfId="4">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="1">
@@ -7905,7 +7862,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="15">
+    <format dxfId="3">
       <pivotArea outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="1">
@@ -8109,17 +8066,17 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{16781676-077F-4238-A45B-27DFF94B5076}" name="evidencija_nastave" displayName="evidencija_nastave" ref="A1:H461" totalsRowShown="0" headerRowDxfId="29" headerRowBorderDxfId="28" tableBorderDxfId="27" totalsRowBorderDxfId="26">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{16781676-077F-4238-A45B-27DFF94B5076}" name="evidencija_nastave" displayName="evidencija_nastave" ref="A1:H461" totalsRowShown="0" headerRowDxfId="17" headerRowBorderDxfId="16" tableBorderDxfId="15" totalsRowBorderDxfId="14">
   <autoFilter ref="A1:H461" xr:uid="{16781676-077F-4238-A45B-27DFF94B5076}"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{50194762-F77D-4094-AA6D-99EE30260FD4}" name="Datum " dataDxfId="25"/>
-    <tableColumn id="8" xr3:uid="{0C577E04-68A0-4F23-BA45-D6CB7CBDAEF9}" name="Odsek" dataDxfId="24"/>
-    <tableColumn id="2" xr3:uid="{7FB038C7-1C51-4E8D-89D6-40EFCD2C3E30}" name="Studijski program" dataDxfId="23"/>
-    <tableColumn id="3" xr3:uid="{42258C3E-B96F-493F-9BC3-C4653A46D16E}" name="Predmet" dataDxfId="22"/>
-    <tableColumn id="7" xr3:uid="{D2E1579F-AC74-46B0-A298-2A297A6F019C}" name="Tip nastave" dataDxfId="21"/>
-    <tableColumn id="4" xr3:uid="{10597A3E-1A4A-4D17-B23F-3033813457E5}" name="Broj časova nastave" dataDxfId="20"/>
-    <tableColumn id="5" xr3:uid="{3E5CD073-EB68-4D84-93A7-166020BE5AA0}" name="Nastavna jedinica" dataDxfId="19"/>
-    <tableColumn id="6" xr3:uid="{9FC5B2DF-EA47-4EFD-A8D3-B4CCE22F5F1B}" name="Broj prisutnih studenata" dataDxfId="18"/>
+    <tableColumn id="1" xr3:uid="{50194762-F77D-4094-AA6D-99EE30260FD4}" name="Datum " dataDxfId="13"/>
+    <tableColumn id="8" xr3:uid="{0C577E04-68A0-4F23-BA45-D6CB7CBDAEF9}" name="Odsek" dataDxfId="12"/>
+    <tableColumn id="2" xr3:uid="{7FB038C7-1C51-4E8D-89D6-40EFCD2C3E30}" name="Studijski program" dataDxfId="11"/>
+    <tableColumn id="3" xr3:uid="{42258C3E-B96F-493F-9BC3-C4653A46D16E}" name="Predmet" dataDxfId="10"/>
+    <tableColumn id="7" xr3:uid="{D2E1579F-AC74-46B0-A298-2A297A6F019C}" name="Tip nastave" dataDxfId="9"/>
+    <tableColumn id="4" xr3:uid="{10597A3E-1A4A-4D17-B23F-3033813457E5}" name="Broj časova nastave" dataDxfId="8"/>
+    <tableColumn id="5" xr3:uid="{3E5CD073-EB68-4D84-93A7-166020BE5AA0}" name="Nastavna jedinica" dataDxfId="7"/>
+    <tableColumn id="6" xr3:uid="{9FC5B2DF-EA47-4EFD-A8D3-B4CCE22F5F1B}" name="Broj prisutnih studenata" dataDxfId="6"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -8462,10 +8419,10 @@
     </row>
     <row r="6" spans="2:6" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
     <row r="7" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="61" t="s">
+      <c r="B7" s="82" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="61"/>
+      <c r="C7" s="82"/>
     </row>
     <row r="8" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B8" s="1" t="s">
@@ -8493,10 +8450,10 @@
       </c>
     </row>
     <row r="12" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B12" s="62" t="s">
+      <c r="B12" s="83" t="s">
         <v>10</v>
       </c>
-      <c r="C12" s="62"/>
+      <c r="C12" s="83"/>
     </row>
     <row r="13" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B13" s="1" t="s">
@@ -8535,10 +8492,10 @@
       <c r="F17" s="4"/>
     </row>
     <row r="18" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B18" s="62" t="s">
+      <c r="B18" s="83" t="s">
         <v>12</v>
       </c>
-      <c r="C18" s="62"/>
+      <c r="C18" s="83"/>
     </row>
     <row r="19" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B19" s="1" t="s">
@@ -8609,10 +8566,10 @@
       <c r="C27" s="1"/>
     </row>
     <row r="29" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B29" s="62" t="s">
+      <c r="B29" s="83" t="s">
         <v>29</v>
       </c>
-      <c r="C29" s="62"/>
+      <c r="C29" s="83"/>
     </row>
     <row r="30" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B30" s="31" t="s">
@@ -8649,10 +8606,10 @@
       <c r="C34" s="1"/>
     </row>
     <row r="37" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B37" s="62" t="s">
+      <c r="B37" s="83" t="s">
         <v>37</v>
       </c>
-      <c r="C37" s="63"/>
+      <c r="C37" s="84"/>
     </row>
     <row r="38" spans="2:3" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B38" s="1" t="s">
@@ -13883,12 +13840,12 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B3" s="64" t="s">
+      <c r="B3" s="85" t="s">
         <v>85</v>
       </c>
-      <c r="C3" s="64"/>
-      <c r="D3" s="64"/>
-      <c r="E3" s="64"/>
+      <c r="C3" s="85"/>
+      <c r="D3" s="85"/>
+      <c r="E3" s="85"/>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.3">
       <c r="C4" s="19" t="s">
@@ -13985,12 +13942,12 @@
       </c>
     </row>
     <row r="22" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B22" s="64" t="s">
+      <c r="B22" s="85" t="s">
         <v>85</v>
       </c>
-      <c r="C22" s="64"/>
-      <c r="D22" s="64"/>
-      <c r="E22" s="64"/>
+      <c r="C22" s="85"/>
+      <c r="D22" s="85"/>
+      <c r="E22" s="85"/>
     </row>
     <row r="23" spans="2:5" x14ac:dyDescent="0.3">
       <c r="C23" s="19" t="s">
@@ -14040,12 +13997,12 @@
       <c r="C30" s="23"/>
     </row>
     <row r="33" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B33" s="64" t="s">
+      <c r="B33" s="85" t="s">
         <v>105</v>
       </c>
-      <c r="C33" s="64"/>
-      <c r="D33" s="64"/>
-      <c r="E33" s="64"/>
+      <c r="C33" s="85"/>
+      <c r="D33" s="85"/>
+      <c r="E33" s="85"/>
     </row>
     <row r="34" spans="2:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C34" s="24" t="s">
@@ -14123,12 +14080,12 @@
     </row>
     <row r="41" spans="2:6" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
     <row r="43" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B43" s="64" t="s">
+      <c r="B43" s="85" t="s">
         <v>118</v>
       </c>
-      <c r="C43" s="64"/>
-      <c r="D43" s="64"/>
-      <c r="E43" s="64"/>
+      <c r="C43" s="85"/>
+      <c r="D43" s="85"/>
+      <c r="E43" s="85"/>
     </row>
     <row r="44" spans="2:6" x14ac:dyDescent="0.3">
       <c r="C44" s="19" t="s">
@@ -14174,10 +14131,10 @@
     </row>
     <row r="51" spans="2:3" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
     <row r="53" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B53" s="64" t="s">
+      <c r="B53" s="85" t="s">
         <v>125</v>
       </c>
-      <c r="C53" s="64"/>
+      <c r="C53" s="85"/>
     </row>
     <row r="54" spans="2:3" x14ac:dyDescent="0.3">
       <c r="C54" s="19" t="s">
@@ -14216,10 +14173,10 @@
     </row>
     <row r="61" spans="2:3" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
     <row r="63" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B63" s="64" t="s">
+      <c r="B63" s="85" t="s">
         <v>119</v>
       </c>
-      <c r="C63" s="64"/>
+      <c r="C63" s="85"/>
     </row>
     <row r="64" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B64" s="41" t="s">
@@ -14323,12 +14280,12 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B3" s="64" t="s">
+      <c r="B3" s="85" t="s">
         <v>85</v>
       </c>
-      <c r="C3" s="64"/>
-      <c r="D3" s="64"/>
-      <c r="E3" s="64"/>
+      <c r="C3" s="85"/>
+      <c r="D3" s="85"/>
+      <c r="E3" s="85"/>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.3">
       <c r="C4" s="19" t="s">
@@ -14424,12 +14381,12 @@
       </c>
     </row>
     <row r="22" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B22" s="64" t="s">
+      <c r="B22" s="85" t="s">
         <v>85</v>
       </c>
-      <c r="C22" s="64"/>
-      <c r="D22" s="64"/>
-      <c r="E22" s="64"/>
+      <c r="C22" s="85"/>
+      <c r="D22" s="85"/>
+      <c r="E22" s="85"/>
     </row>
     <row r="23" spans="2:5" x14ac:dyDescent="0.3">
       <c r="C23" s="19" t="s">
@@ -14481,12 +14438,12 @@
       </c>
     </row>
     <row r="33" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B33" s="64" t="s">
+      <c r="B33" s="85" t="s">
         <v>105</v>
       </c>
-      <c r="C33" s="64"/>
-      <c r="D33" s="64"/>
-      <c r="E33" s="64"/>
+      <c r="C33" s="85"/>
+      <c r="D33" s="85"/>
+      <c r="E33" s="85"/>
     </row>
     <row r="34" spans="2:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C34" s="24" t="s">
@@ -14549,12 +14506,12 @@
       <c r="E40" s="3"/>
     </row>
     <row r="43" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B43" s="64" t="s">
+      <c r="B43" s="85" t="s">
         <v>118</v>
       </c>
-      <c r="C43" s="64"/>
-      <c r="D43" s="64"/>
-      <c r="E43" s="64"/>
+      <c r="C43" s="85"/>
+      <c r="D43" s="85"/>
+      <c r="E43" s="85"/>
     </row>
     <row r="44" spans="2:6" x14ac:dyDescent="0.3">
       <c r="C44" s="19" t="s">
@@ -14611,10 +14568,10 @@
       <c r="C52" s="3"/>
     </row>
     <row r="55" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B55" s="64" t="s">
+      <c r="B55" s="85" t="s">
         <v>125</v>
       </c>
-      <c r="C55" s="64"/>
+      <c r="C55" s="85"/>
     </row>
     <row r="56" spans="2:3" x14ac:dyDescent="0.3">
       <c r="C56" s="19" t="s">
@@ -14652,10 +14609,10 @@
       <c r="C62" s="3"/>
     </row>
     <row r="65" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B65" s="64" t="s">
+      <c r="B65" s="85" t="s">
         <v>119</v>
       </c>
-      <c r="C65" s="64"/>
+      <c r="C65" s="85"/>
     </row>
     <row r="66" spans="2:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B66" s="41" t="s">
@@ -14779,12 +14736,12 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B3" s="64" t="s">
+      <c r="B3" s="85" t="s">
         <v>85</v>
       </c>
-      <c r="C3" s="64"/>
-      <c r="D3" s="64"/>
-      <c r="E3" s="64"/>
+      <c r="C3" s="85"/>
+      <c r="D3" s="85"/>
+      <c r="E3" s="85"/>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.3">
       <c r="C4" s="19" t="s">
@@ -14880,12 +14837,12 @@
       </c>
     </row>
     <row r="22" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B22" s="64" t="s">
+      <c r="B22" s="85" t="s">
         <v>85</v>
       </c>
-      <c r="C22" s="64"/>
-      <c r="D22" s="64"/>
-      <c r="E22" s="64"/>
+      <c r="C22" s="85"/>
+      <c r="D22" s="85"/>
+      <c r="E22" s="85"/>
     </row>
     <row r="23" spans="2:5" x14ac:dyDescent="0.3">
       <c r="C23" s="19" t="s">
@@ -14945,12 +14902,12 @@
       </c>
     </row>
     <row r="33" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B33" s="64" t="s">
+      <c r="B33" s="85" t="s">
         <v>105</v>
       </c>
-      <c r="C33" s="64"/>
-      <c r="D33" s="64"/>
-      <c r="E33" s="64"/>
+      <c r="C33" s="85"/>
+      <c r="D33" s="85"/>
+      <c r="E33" s="85"/>
     </row>
     <row r="34" spans="2:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C34" s="24" t="s">
@@ -15009,12 +14966,12 @@
       <c r="E40" s="3"/>
     </row>
     <row r="43" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B43" s="64" t="s">
+      <c r="B43" s="85" t="s">
         <v>118</v>
       </c>
-      <c r="C43" s="64"/>
-      <c r="D43" s="64"/>
-      <c r="E43" s="64"/>
+      <c r="C43" s="85"/>
+      <c r="D43" s="85"/>
+      <c r="E43" s="85"/>
     </row>
     <row r="44" spans="2:6" x14ac:dyDescent="0.3">
       <c r="C44" s="19" t="s">
@@ -15111,10 +15068,10 @@
       <c r="C58" s="3"/>
     </row>
     <row r="61" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B61" s="64" t="s">
+      <c r="B61" s="85" t="s">
         <v>125</v>
       </c>
-      <c r="C61" s="64"/>
+      <c r="C61" s="85"/>
     </row>
     <row r="62" spans="2:3" x14ac:dyDescent="0.3">
       <c r="C62" s="19" t="s">
@@ -15154,10 +15111,10 @@
       <c r="C68" s="3"/>
     </row>
     <row r="71" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B71" s="64" t="s">
+      <c r="B71" s="85" t="s">
         <v>119</v>
       </c>
-      <c r="C71" s="64"/>
+      <c r="C71" s="85"/>
     </row>
     <row r="72" spans="2:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B72" s="41" t="s">
@@ -15333,12 +15290,12 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B3" s="64" t="s">
+      <c r="B3" s="85" t="s">
         <v>85</v>
       </c>
-      <c r="C3" s="64"/>
-      <c r="D3" s="64"/>
-      <c r="E3" s="64"/>
+      <c r="C3" s="85"/>
+      <c r="D3" s="85"/>
+      <c r="E3" s="85"/>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.3">
       <c r="C4" s="19" t="s">
@@ -15434,12 +15391,12 @@
       </c>
     </row>
     <row r="22" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B22" s="64" t="s">
+      <c r="B22" s="85" t="s">
         <v>85</v>
       </c>
-      <c r="C22" s="64"/>
-      <c r="D22" s="64"/>
-      <c r="E22" s="64"/>
+      <c r="C22" s="85"/>
+      <c r="D22" s="85"/>
+      <c r="E22" s="85"/>
     </row>
     <row r="23" spans="2:5" x14ac:dyDescent="0.3">
       <c r="C23" s="19" t="s">
@@ -15489,12 +15446,12 @@
       </c>
     </row>
     <row r="32" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B32" s="64" t="s">
+      <c r="B32" s="85" t="s">
         <v>105</v>
       </c>
-      <c r="C32" s="64"/>
-      <c r="D32" s="64"/>
-      <c r="E32" s="64"/>
+      <c r="C32" s="85"/>
+      <c r="D32" s="85"/>
+      <c r="E32" s="85"/>
     </row>
     <row r="33" spans="2:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C33" s="24" t="s">
@@ -15555,12 +15512,12 @@
       <c r="E39" s="3"/>
     </row>
     <row r="42" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B42" s="64" t="s">
+      <c r="B42" s="85" t="s">
         <v>118</v>
       </c>
-      <c r="C42" s="64"/>
-      <c r="D42" s="64"/>
-      <c r="E42" s="64"/>
+      <c r="C42" s="85"/>
+      <c r="D42" s="85"/>
+      <c r="E42" s="85"/>
     </row>
     <row r="43" spans="2:6" x14ac:dyDescent="0.3">
       <c r="C43" s="19" t="s">
@@ -15657,10 +15614,10 @@
       <c r="C57" s="3"/>
     </row>
     <row r="60" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B60" s="64" t="s">
+      <c r="B60" s="85" t="s">
         <v>125</v>
       </c>
-      <c r="C60" s="64"/>
+      <c r="C60" s="85"/>
     </row>
     <row r="61" spans="2:3" x14ac:dyDescent="0.3">
       <c r="C61" s="19" t="s">
@@ -15700,10 +15657,10 @@
       <c r="C67" s="3"/>
     </row>
     <row r="70" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B70" s="64" t="s">
+      <c r="B70" s="85" t="s">
         <v>119</v>
       </c>
-      <c r="C70" s="64"/>
+      <c r="C70" s="85"/>
     </row>
     <row r="71" spans="2:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B71" s="41" t="s">
@@ -15856,8 +15813,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2EB64B95-66F9-4F12-9234-061A62D7269E}">
   <dimension ref="A4:K26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B3" workbookViewId="0">
-      <selection activeCell="M20" sqref="M20"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="108" zoomScaleNormal="71" workbookViewId="0">
+      <selection activeCell="M16" sqref="M16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -15885,318 +15842,318 @@
       <c r="F4" s="55"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B6" s="65" t="s">
+      <c r="B6" s="61" t="s">
         <v>196</v>
       </c>
-      <c r="C6" s="65" t="s">
+      <c r="C6" s="61" t="s">
         <v>197</v>
       </c>
-      <c r="D6" s="66"/>
-      <c r="E6" s="67"/>
-      <c r="J6" s="65" t="s">
+      <c r="D6" s="62"/>
+      <c r="E6" s="63"/>
+      <c r="J6" s="61" t="s">
         <v>198</v>
       </c>
-      <c r="K6" s="70" t="s">
+      <c r="K6" s="66" t="s">
         <v>199</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B7" s="65" t="s">
+      <c r="B7" s="61" t="s">
         <v>198</v>
       </c>
-      <c r="C7" s="68" t="s">
+      <c r="C7" s="64" t="s">
         <v>56</v>
       </c>
-      <c r="D7" s="69" t="s">
+      <c r="D7" s="65" t="s">
         <v>200</v>
       </c>
-      <c r="E7" s="70" t="s">
+      <c r="E7" s="66" t="s">
         <v>201</v>
       </c>
-      <c r="J7" s="71" t="s">
+      <c r="J7" s="67" t="s">
         <v>54</v>
       </c>
-      <c r="K7" s="86"/>
+      <c r="K7" s="79"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B8" s="71" t="s">
+      <c r="B8" s="67" t="s">
         <v>54</v>
       </c>
-      <c r="C8" s="72"/>
-      <c r="D8" s="73"/>
-      <c r="E8" s="74"/>
-      <c r="J8" s="75" t="s">
+      <c r="C8" s="64"/>
+      <c r="D8" s="65"/>
+      <c r="E8" s="66"/>
+      <c r="J8" s="68" t="s">
         <v>202</v>
       </c>
-      <c r="K8" s="87"/>
+      <c r="K8" s="80"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B9" s="75" t="s">
+      <c r="B9" s="68" t="s">
         <v>202</v>
       </c>
-      <c r="C9" s="76"/>
-      <c r="D9" s="77"/>
-      <c r="E9" s="78"/>
-      <c r="J9" s="79" t="s">
+      <c r="C9" s="69"/>
+      <c r="D9" s="70"/>
+      <c r="E9" s="71"/>
+      <c r="J9" s="72" t="s">
         <v>204</v>
       </c>
-      <c r="K9" s="87"/>
+      <c r="K9" s="80"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B10" s="79" t="s">
+      <c r="B10" s="72" t="s">
         <v>204</v>
       </c>
-      <c r="C10" s="76"/>
-      <c r="D10" s="77"/>
-      <c r="E10" s="78"/>
-      <c r="J10" s="80" t="s">
+      <c r="C10" s="69"/>
+      <c r="D10" s="70"/>
+      <c r="E10" s="71"/>
+      <c r="J10" s="73" t="s">
         <v>16</v>
       </c>
-      <c r="K10" s="87">
+      <c r="K10" s="80">
         <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B11" s="80" t="s">
+      <c r="B11" s="73" t="s">
         <v>16</v>
       </c>
-      <c r="C11" s="76">
+      <c r="C11" s="69">
         <v>2</v>
       </c>
-      <c r="D11" s="77">
+      <c r="D11" s="70">
         <v>2</v>
       </c>
-      <c r="E11" s="78">
+      <c r="E11" s="71">
         <v>4</v>
       </c>
-      <c r="J11" s="80" t="s">
+      <c r="J11" s="73" t="s">
         <v>59</v>
       </c>
-      <c r="K11" s="87">
+      <c r="K11" s="80">
         <v>11.333333333333334</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B12" s="80" t="s">
+      <c r="B12" s="73" t="s">
         <v>59</v>
       </c>
-      <c r="C12" s="76">
+      <c r="C12" s="69">
         <v>2</v>
       </c>
-      <c r="D12" s="77">
+      <c r="D12" s="70">
         <v>4</v>
       </c>
-      <c r="E12" s="78">
+      <c r="E12" s="71">
         <v>6</v>
       </c>
-      <c r="J12" s="75" t="s">
+      <c r="J12" s="68" t="s">
         <v>203</v>
       </c>
-      <c r="K12" s="87"/>
+      <c r="K12" s="80"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B13" s="75" t="s">
+      <c r="B13" s="68" t="s">
         <v>203</v>
       </c>
-      <c r="C13" s="76"/>
-      <c r="D13" s="77"/>
-      <c r="E13" s="78"/>
-      <c r="J13" s="79" t="s">
+      <c r="C13" s="69"/>
+      <c r="D13" s="70"/>
+      <c r="E13" s="71"/>
+      <c r="J13" s="72" t="s">
         <v>205</v>
       </c>
-      <c r="K13" s="87"/>
+      <c r="K13" s="80"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B14" s="79" t="s">
+      <c r="B14" s="72" t="s">
         <v>205</v>
       </c>
-      <c r="C14" s="76"/>
-      <c r="D14" s="77"/>
-      <c r="E14" s="78"/>
-      <c r="J14" s="80" t="s">
+      <c r="C14" s="69"/>
+      <c r="D14" s="70"/>
+      <c r="E14" s="71"/>
+      <c r="J14" s="73" t="s">
         <v>16</v>
       </c>
-      <c r="K14" s="87">
+      <c r="K14" s="80">
         <v>34.5</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B15" s="80" t="s">
+      <c r="B15" s="73" t="s">
         <v>16</v>
       </c>
-      <c r="C15" s="76">
+      <c r="C15" s="69">
         <v>8</v>
       </c>
-      <c r="D15" s="77"/>
-      <c r="E15" s="78">
+      <c r="D15" s="70"/>
+      <c r="E15" s="71">
         <v>8</v>
       </c>
-      <c r="J15" s="80" t="s">
+      <c r="J15" s="73" t="s">
         <v>59</v>
       </c>
-      <c r="K15" s="87">
+      <c r="K15" s="80">
         <v>32.75</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B16" s="80" t="s">
+      <c r="B16" s="73" t="s">
         <v>59</v>
       </c>
-      <c r="C16" s="76">
+      <c r="C16" s="69">
         <v>8</v>
       </c>
-      <c r="D16" s="77"/>
-      <c r="E16" s="78">
+      <c r="D16" s="70"/>
+      <c r="E16" s="71">
         <v>8</v>
       </c>
-      <c r="J16" s="79" t="s">
+      <c r="J16" s="72" t="s">
         <v>206</v>
       </c>
-      <c r="K16" s="87"/>
+      <c r="K16" s="80"/>
     </row>
     <row r="17" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B17" s="79" t="s">
+      <c r="B17" s="72" t="s">
         <v>206</v>
       </c>
-      <c r="C17" s="76"/>
-      <c r="D17" s="77"/>
-      <c r="E17" s="78"/>
-      <c r="J17" s="80" t="s">
+      <c r="C17" s="69"/>
+      <c r="D17" s="70"/>
+      <c r="E17" s="71"/>
+      <c r="J17" s="73" t="s">
         <v>16</v>
       </c>
-      <c r="K17" s="87">
+      <c r="K17" s="80">
         <v>30.75</v>
       </c>
     </row>
     <row r="18" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B18" s="80" t="s">
+      <c r="B18" s="73" t="s">
         <v>16</v>
       </c>
-      <c r="C18" s="76">
+      <c r="C18" s="69">
         <v>6</v>
       </c>
-      <c r="D18" s="77">
+      <c r="D18" s="70">
         <v>2</v>
       </c>
-      <c r="E18" s="78">
+      <c r="E18" s="71">
         <v>8</v>
       </c>
-      <c r="J18" s="80" t="s">
+      <c r="J18" s="73" t="s">
         <v>59</v>
       </c>
-      <c r="K18" s="87">
+      <c r="K18" s="80">
         <v>17.8</v>
       </c>
     </row>
     <row r="19" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B19" s="80" t="s">
+      <c r="B19" s="73" t="s">
         <v>59</v>
       </c>
-      <c r="C19" s="76">
+      <c r="C19" s="69">
         <v>8</v>
       </c>
-      <c r="D19" s="77">
+      <c r="D19" s="70">
         <v>4</v>
       </c>
-      <c r="E19" s="78">
+      <c r="E19" s="71">
         <v>12</v>
       </c>
-      <c r="J19" s="79" t="s">
+      <c r="J19" s="72" t="s">
         <v>207</v>
       </c>
-      <c r="K19" s="87"/>
+      <c r="K19" s="80"/>
     </row>
     <row r="20" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B20" s="79" t="s">
+      <c r="B20" s="72" t="s">
         <v>207</v>
       </c>
-      <c r="C20" s="76"/>
-      <c r="D20" s="77"/>
-      <c r="E20" s="78"/>
-      <c r="J20" s="80" t="s">
+      <c r="C20" s="69"/>
+      <c r="D20" s="70"/>
+      <c r="E20" s="71"/>
+      <c r="J20" s="73" t="s">
         <v>16</v>
       </c>
-      <c r="K20" s="87">
+      <c r="K20" s="80">
         <v>36</v>
       </c>
     </row>
     <row r="21" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B21" s="80" t="s">
+      <c r="B21" s="73" t="s">
         <v>16</v>
       </c>
-      <c r="C21" s="76">
+      <c r="C21" s="69">
         <v>9</v>
       </c>
-      <c r="D21" s="77"/>
-      <c r="E21" s="78">
+      <c r="D21" s="70"/>
+      <c r="E21" s="71">
         <v>9</v>
       </c>
-      <c r="J21" s="80" t="s">
+      <c r="J21" s="73" t="s">
         <v>59</v>
       </c>
-      <c r="K21" s="87">
+      <c r="K21" s="80">
         <v>24</v>
       </c>
     </row>
     <row r="22" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B22" s="80" t="s">
+      <c r="B22" s="73" t="s">
         <v>59</v>
       </c>
-      <c r="C22" s="76">
+      <c r="C22" s="69">
         <v>8</v>
       </c>
-      <c r="D22" s="77"/>
-      <c r="E22" s="78">
+      <c r="D22" s="70"/>
+      <c r="E22" s="71">
         <v>8</v>
       </c>
-      <c r="J22" s="81" t="s">
+      <c r="J22" s="74" t="s">
         <v>200</v>
       </c>
-      <c r="K22" s="87"/>
+      <c r="K22" s="80"/>
     </row>
     <row r="23" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B23" s="81" t="s">
+      <c r="B23" s="74" t="s">
         <v>200</v>
       </c>
-      <c r="C23" s="76"/>
-      <c r="D23" s="77"/>
-      <c r="E23" s="78"/>
-      <c r="J23" s="75" t="s">
+      <c r="C23" s="69"/>
+      <c r="D23" s="70"/>
+      <c r="E23" s="71"/>
+      <c r="J23" s="68" t="s">
         <v>595</v>
       </c>
-      <c r="K23" s="87"/>
+      <c r="K23" s="80"/>
     </row>
     <row r="24" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B24" s="75" t="s">
+      <c r="B24" s="68" t="s">
         <v>595</v>
       </c>
-      <c r="C24" s="76"/>
-      <c r="D24" s="77"/>
-      <c r="E24" s="78"/>
-      <c r="J24" s="79" t="s">
+      <c r="C24" s="69"/>
+      <c r="D24" s="70"/>
+      <c r="E24" s="71"/>
+      <c r="J24" s="72" t="s">
         <v>595</v>
       </c>
-      <c r="K24" s="87"/>
+      <c r="K24" s="80"/>
     </row>
     <row r="25" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B25" s="79" t="s">
+      <c r="B25" s="72" t="s">
         <v>595</v>
       </c>
-      <c r="C25" s="76"/>
-      <c r="D25" s="77"/>
-      <c r="E25" s="78"/>
-      <c r="J25" s="82" t="s">
+      <c r="C25" s="69"/>
+      <c r="D25" s="70"/>
+      <c r="E25" s="71"/>
+      <c r="J25" s="75" t="s">
         <v>200</v>
       </c>
-      <c r="K25" s="88"/>
+      <c r="K25" s="81"/>
     </row>
     <row r="26" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B26" s="82" t="s">
+      <c r="B26" s="75" t="s">
         <v>200</v>
       </c>
-      <c r="C26" s="83"/>
-      <c r="D26" s="84"/>
-      <c r="E26" s="85"/>
+      <c r="C26" s="76"/>
+      <c r="D26" s="77"/>
+      <c r="E26" s="78"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>